<commit_message>
forREnd(8) 改为 forREnd, ifREnd(6) 改为 ifREnd
</commit_message>
<xml_diff>
--- a/test/report.xlsx
+++ b/test/report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>&lt;%=_data_[0][0].table_name%&gt;</t>
   </si>
@@ -76,15 +76,10 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;%forREnd(8)%&gt;</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;%forRBegin rs1,i in _data_[1]%&gt;</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>这个(8)代表forRBegin跟forREnd标签直接有8行 行号11 - 行号3 = 8</t>
+  </si>
+  <si>
+    <t>&lt;%forREnd%&gt;</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -713,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -773,7 +768,7 @@
     </row>
     <row r="3" spans="1:17" ht="28.5" customHeight="1">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -896,14 +891,9 @@
     </row>
     <row r="11" spans="1:17" ht="18.95" customHeight="1">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" s="17"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>